<commit_message>
Edit and ehance map in pandas
</commit_message>
<xml_diff>
--- a/BDI302c_FINAL-UP_FUMM.xlsx
+++ b/BDI302c_FINAL-UP_FUMM.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="BDI302c_FINAL-UP_FUMM" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Class</t>
   </si>
@@ -34,28 +34,94 @@
     <t>A18C.DS</t>
   </si>
   <si>
-    <t>QE180047</t>
-  </si>
-  <si>
-    <t>QE180049</t>
-  </si>
-  <si>
-    <t>QE180050</t>
-  </si>
-  <si>
-    <t>QE180051</t>
-  </si>
-  <si>
-    <t>Cao Ngọc Ý</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>Trần Thị B</t>
-  </si>
-  <si>
-    <t>Lê Thị C</t>
+    <t>QE180001</t>
+  </si>
+  <si>
+    <t>QE180002</t>
+  </si>
+  <si>
+    <t>QE180003</t>
+  </si>
+  <si>
+    <t>QE180004</t>
+  </si>
+  <si>
+    <t>QE180005</t>
+  </si>
+  <si>
+    <t>QE180006</t>
+  </si>
+  <si>
+    <t>QE180007</t>
+  </si>
+  <si>
+    <t>QE180008</t>
+  </si>
+  <si>
+    <t>QE180009</t>
+  </si>
+  <si>
+    <t>QE180010</t>
+  </si>
+  <si>
+    <t>QE180011</t>
+  </si>
+  <si>
+    <t>QE180012</t>
+  </si>
+  <si>
+    <t>QE180013</t>
+  </si>
+  <si>
+    <t>QE180014</t>
+  </si>
+  <si>
+    <t>QE180015</t>
+  </si>
+  <si>
+    <t>Student 1</t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Student 4</t>
+  </si>
+  <si>
+    <t>Student 5</t>
+  </si>
+  <si>
+    <t>Student 6</t>
+  </si>
+  <si>
+    <t>Student 7</t>
+  </si>
+  <si>
+    <t>Student 8</t>
+  </si>
+  <si>
+    <t>Student 9</t>
+  </si>
+  <si>
+    <t>Student 10</t>
+  </si>
+  <si>
+    <t>Student 11</t>
+  </si>
+  <si>
+    <t>Student 12</t>
+  </si>
+  <si>
+    <t>Student 13</t>
+  </si>
+  <si>
+    <t>Student 14</t>
+  </si>
+  <si>
+    <t>Student 15</t>
   </si>
 </sst>
 </file>
@@ -413,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +510,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>9.33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -458,10 +521,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>9.73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -472,10 +532,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>8.5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -486,10 +543,128 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>7.8</v>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>